<commit_message>
added blue ammonia choice added new fuel costs
</commit_message>
<xml_diff>
--- a/data/existing_fleet.xlsx
+++ b/data/existing_fleet.xlsx
@@ -9,13 +9,13 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="13500" firstSheet="1" activeTab="3"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="13500" firstSheet="1" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="11" r:id="rId1"/>
     <sheet name="ships" sheetId="10" r:id="rId2"/>
     <sheet name="Preexisting fleet stats" sheetId="1" r:id="rId3"/>
-    <sheet name="MFO fleet" sheetId="2" r:id="rId4"/>
+    <sheet name="MDO fleet" sheetId="2" r:id="rId4"/>
     <sheet name="Scrubber fleet" sheetId="3" r:id="rId5"/>
     <sheet name="LNG fleet" sheetId="4" r:id="rId6"/>
     <sheet name="Battery fleet" sheetId="5" r:id="rId7"/>
@@ -318,21 +318,6 @@
     <t>T_HYD</t>
   </si>
   <si>
-    <t>"T_MFO"</t>
-  </si>
-  <si>
-    <t>"B_MFO"</t>
-  </si>
-  <si>
-    <t>"G_MFO"</t>
-  </si>
-  <si>
-    <t>"C_MFO"</t>
-  </si>
-  <si>
-    <t>"O_MFO"</t>
-  </si>
-  <si>
     <t>"T_SCR"</t>
   </si>
   <si>
@@ -439,6 +424,21 @@
   </si>
   <si>
     <t>test</t>
+  </si>
+  <si>
+    <t>"T_MDO"</t>
+  </si>
+  <si>
+    <t>"B_MDO"</t>
+  </si>
+  <si>
+    <t>"G_MDO"</t>
+  </si>
+  <si>
+    <t>"C_MDO"</t>
+  </si>
+  <si>
+    <t>"O_MDO"</t>
   </si>
 </sst>
 </file>
@@ -2209,22 +2209,22 @@
         <v>27</v>
       </c>
       <c r="D2" t="s">
-        <v>129</v>
+        <v>124</v>
       </c>
       <c r="E2" t="s">
-        <v>130</v>
+        <v>125</v>
       </c>
       <c r="F2" t="s">
-        <v>129</v>
+        <v>124</v>
       </c>
       <c r="G2" t="s">
-        <v>131</v>
+        <v>126</v>
       </c>
       <c r="H2" t="s">
-        <v>132</v>
+        <v>127</v>
       </c>
       <c r="I2" t="s">
-        <v>133</v>
+        <v>128</v>
       </c>
     </row>
     <row r="3" spans="2:9">
@@ -4480,23 +4480,23 @@
         <v>2011</v>
       </c>
       <c r="C4">
-        <f>+'MFO fleet'!C6</f>
+        <f>+'MDO fleet'!C6</f>
         <v>10603</v>
       </c>
       <c r="D4">
-        <f>+'MFO fleet'!D6</f>
+        <f>+'MDO fleet'!D6</f>
         <v>8223</v>
       </c>
       <c r="E4">
-        <f>+'MFO fleet'!E6</f>
+        <f>+'MDO fleet'!E6</f>
         <v>21085</v>
       </c>
       <c r="F4">
-        <f>+'MFO fleet'!F6</f>
+        <f>+'MDO fleet'!F6</f>
         <v>4963</v>
       </c>
       <c r="G4">
-        <f>+'MFO fleet'!G6</f>
+        <f>+'MDO fleet'!G6</f>
         <v>38352</v>
       </c>
       <c r="H4">
@@ -4626,23 +4626,23 @@
         <v>2012</v>
       </c>
       <c r="C5">
-        <f>+'MFO fleet'!C7</f>
+        <f>+'MDO fleet'!C7</f>
         <v>8828</v>
       </c>
       <c r="D5">
-        <f>+'MFO fleet'!D7</f>
+        <f>+'MDO fleet'!D7</f>
         <v>8993</v>
       </c>
       <c r="E5">
-        <f>+'MFO fleet'!E7</f>
+        <f>+'MDO fleet'!E7</f>
         <v>20302</v>
       </c>
       <c r="F5">
-        <f>+'MFO fleet'!F7</f>
+        <f>+'MDO fleet'!F7</f>
         <v>5090</v>
       </c>
       <c r="G5">
-        <f>+'MFO fleet'!G7</f>
+        <f>+'MDO fleet'!G7</f>
         <v>41410</v>
       </c>
       <c r="H5">
@@ -4772,23 +4772,23 @@
         <v>2013</v>
       </c>
       <c r="C6">
-        <f>+'MFO fleet'!C8</f>
+        <f>+'MDO fleet'!C8</f>
         <v>9017</v>
       </c>
       <c r="D6">
-        <f>+'MFO fleet'!D8</f>
+        <f>+'MDO fleet'!D8</f>
         <v>9550</v>
       </c>
       <c r="E6">
-        <f>+'MFO fleet'!E8</f>
+        <f>+'MDO fleet'!E8</f>
         <v>20271</v>
       </c>
       <c r="F6">
-        <f>+'MFO fleet'!F8</f>
+        <f>+'MDO fleet'!F8</f>
         <v>5096</v>
       </c>
       <c r="G6">
-        <f>+'MFO fleet'!G8</f>
+        <f>+'MDO fleet'!G8</f>
         <v>42404</v>
       </c>
       <c r="H6">
@@ -4918,23 +4918,23 @@
         <v>2014</v>
       </c>
       <c r="C7">
-        <f>+'MFO fleet'!C9</f>
+        <f>+'MDO fleet'!C9</f>
         <v>9210</v>
       </c>
       <c r="D7">
-        <f>+'MFO fleet'!D9</f>
+        <f>+'MDO fleet'!D9</f>
         <v>10120</v>
       </c>
       <c r="E7">
-        <f>+'MFO fleet'!E9</f>
+        <f>+'MDO fleet'!E9</f>
         <v>19644</v>
       </c>
       <c r="F7">
-        <f>+'MFO fleet'!F9</f>
+        <f>+'MDO fleet'!F9</f>
         <v>5074</v>
       </c>
       <c r="G7">
-        <f>+'MFO fleet'!G9</f>
+        <f>+'MDO fleet'!G9</f>
         <v>43659</v>
       </c>
       <c r="H7">
@@ -5064,23 +5064,23 @@
         <v>2015</v>
       </c>
       <c r="C8">
-        <f>+'MFO fleet'!C10</f>
+        <f>+'MDO fleet'!C10</f>
         <v>9639</v>
       </c>
       <c r="D8">
-        <f>+'MFO fleet'!D10</f>
+        <f>+'MDO fleet'!D10</f>
         <v>10421</v>
       </c>
       <c r="E8">
-        <f>+'MFO fleet'!E10</f>
+        <f>+'MDO fleet'!E10</f>
         <v>19530</v>
       </c>
       <c r="F8">
-        <f>+'MFO fleet'!F10</f>
+        <f>+'MDO fleet'!F10</f>
         <v>5055</v>
       </c>
       <c r="G8">
-        <f>+'MFO fleet'!G10</f>
+        <f>+'MDO fleet'!G10</f>
         <v>45413</v>
       </c>
       <c r="H8">
@@ -5210,23 +5210,23 @@
         <v>2016</v>
       </c>
       <c r="C9">
-        <f>+'MFO fleet'!C11</f>
+        <f>+'MDO fleet'!C11</f>
         <v>9864</v>
       </c>
       <c r="D9">
-        <f>+'MFO fleet'!D11</f>
+        <f>+'MDO fleet'!D11</f>
         <v>10634</v>
       </c>
       <c r="E9">
-        <f>+'MFO fleet'!E11</f>
+        <f>+'MDO fleet'!E11</f>
         <v>19652</v>
       </c>
       <c r="F9">
-        <f>+'MFO fleet'!F11</f>
+        <f>+'MDO fleet'!F11</f>
         <v>5155</v>
       </c>
       <c r="G9">
-        <f>+'MFO fleet'!G11</f>
+        <f>+'MDO fleet'!G11</f>
         <v>46242</v>
       </c>
       <c r="H9">
@@ -5356,23 +5356,23 @@
         <v>2017</v>
       </c>
       <c r="C10">
-        <f>+'MFO fleet'!C12</f>
+        <f>+'MDO fleet'!C12</f>
         <v>10129</v>
       </c>
       <c r="D10">
-        <f>+'MFO fleet'!D12</f>
+        <f>+'MDO fleet'!D12</f>
         <v>10752</v>
       </c>
       <c r="E10">
-        <f>+'MFO fleet'!E12</f>
+        <f>+'MDO fleet'!E12</f>
         <v>19660</v>
       </c>
       <c r="F10">
-        <f>+'MFO fleet'!F12</f>
+        <f>+'MDO fleet'!F12</f>
         <v>5069</v>
       </c>
       <c r="G10">
-        <f>+'MFO fleet'!G12</f>
+        <f>+'MDO fleet'!G12</f>
         <v>47001</v>
       </c>
       <c r="H10">
@@ -5502,23 +5502,23 @@
         <v>2018</v>
       </c>
       <c r="C11">
-        <f>+'MFO fleet'!C13</f>
+        <f>+'MDO fleet'!C13</f>
         <v>10274</v>
       </c>
       <c r="D11">
-        <f>+'MFO fleet'!D13</f>
+        <f>+'MDO fleet'!D13</f>
         <v>10872</v>
       </c>
       <c r="E11">
-        <f>+'MFO fleet'!E13</f>
+        <f>+'MDO fleet'!E13</f>
         <v>19520</v>
       </c>
       <c r="F11">
-        <f>+'MFO fleet'!F13</f>
+        <f>+'MDO fleet'!F13</f>
         <v>5006</v>
       </c>
       <c r="G11">
-        <f>+'MFO fleet'!G13</f>
+        <f>+'MDO fleet'!G13</f>
         <v>47450</v>
       </c>
       <c r="H11">
@@ -5648,23 +5648,23 @@
         <v>2019</v>
       </c>
       <c r="C12">
-        <f>+'MFO fleet'!C14</f>
+        <f>+'MDO fleet'!C14</f>
         <v>10226</v>
       </c>
       <c r="D12">
-        <f>+'MFO fleet'!D14</f>
+        <f>+'MDO fleet'!D14</f>
         <v>10318</v>
       </c>
       <c r="E12">
-        <f>+'MFO fleet'!E14</f>
+        <f>+'MDO fleet'!E14</f>
         <v>18659</v>
       </c>
       <c r="F12">
-        <f>+'MFO fleet'!F14</f>
+        <f>+'MDO fleet'!F14</f>
         <v>4618</v>
       </c>
       <c r="G12">
-        <f>+'MFO fleet'!G14</f>
+        <f>+'MDO fleet'!G14</f>
         <v>48919</v>
       </c>
       <c r="H12">
@@ -5794,23 +5794,23 @@
         <v>2020</v>
       </c>
       <c r="C13">
-        <f>+'MFO fleet'!C15</f>
+        <f>+'MDO fleet'!C15</f>
         <v>0</v>
       </c>
       <c r="D13">
-        <f>+'MFO fleet'!D15</f>
+        <f>+'MDO fleet'!D15</f>
         <v>0</v>
       </c>
       <c r="E13">
-        <f>+'MFO fleet'!E15</f>
+        <f>+'MDO fleet'!E15</f>
         <v>0</v>
       </c>
       <c r="F13">
-        <f>+'MFO fleet'!F15</f>
+        <f>+'MDO fleet'!F15</f>
         <v>0</v>
       </c>
       <c r="G13">
-        <f>+'MFO fleet'!G15</f>
+        <f>+'MDO fleet'!G15</f>
         <v>0</v>
       </c>
       <c r="H13">
@@ -5940,23 +5940,23 @@
         <v>2021</v>
       </c>
       <c r="C14">
-        <f>+'MFO fleet'!C16</f>
+        <f>+'MDO fleet'!C16</f>
         <v>0</v>
       </c>
       <c r="D14">
-        <f>+'MFO fleet'!D16</f>
+        <f>+'MDO fleet'!D16</f>
         <v>0</v>
       </c>
       <c r="E14">
-        <f>+'MFO fleet'!E16</f>
+        <f>+'MDO fleet'!E16</f>
         <v>0</v>
       </c>
       <c r="F14">
-        <f>+'MFO fleet'!F16</f>
+        <f>+'MDO fleet'!F16</f>
         <v>0</v>
       </c>
       <c r="G14">
-        <f>+'MFO fleet'!G16</f>
+        <f>+'MDO fleet'!G16</f>
         <v>0</v>
       </c>
       <c r="H14">
@@ -6086,23 +6086,23 @@
         <v>2022</v>
       </c>
       <c r="C15">
-        <f>+'MFO fleet'!C17</f>
+        <f>+'MDO fleet'!C17</f>
         <v>0</v>
       </c>
       <c r="D15">
-        <f>+'MFO fleet'!D17</f>
+        <f>+'MDO fleet'!D17</f>
         <v>0</v>
       </c>
       <c r="E15">
-        <f>+'MFO fleet'!E17</f>
+        <f>+'MDO fleet'!E17</f>
         <v>0</v>
       </c>
       <c r="F15">
-        <f>+'MFO fleet'!F17</f>
+        <f>+'MDO fleet'!F17</f>
         <v>0</v>
       </c>
       <c r="G15">
-        <f>+'MFO fleet'!G17</f>
+        <f>+'MDO fleet'!G17</f>
         <v>0</v>
       </c>
       <c r="H15">
@@ -6232,23 +6232,23 @@
         <v>2023</v>
       </c>
       <c r="C16">
-        <f>+'MFO fleet'!C18</f>
+        <f>+'MDO fleet'!C18</f>
         <v>0</v>
       </c>
       <c r="D16">
-        <f>+'MFO fleet'!D18</f>
+        <f>+'MDO fleet'!D18</f>
         <v>0</v>
       </c>
       <c r="E16">
-        <f>+'MFO fleet'!E18</f>
+        <f>+'MDO fleet'!E18</f>
         <v>0</v>
       </c>
       <c r="F16">
-        <f>+'MFO fleet'!F18</f>
+        <f>+'MDO fleet'!F18</f>
         <v>0</v>
       </c>
       <c r="G16">
-        <f>+'MFO fleet'!G18</f>
+        <f>+'MDO fleet'!G18</f>
         <v>0</v>
       </c>
       <c r="H16">
@@ -6378,23 +6378,23 @@
         <v>2024</v>
       </c>
       <c r="C17">
-        <f>+'MFO fleet'!C19</f>
+        <f>+'MDO fleet'!C19</f>
         <v>0</v>
       </c>
       <c r="D17">
-        <f>+'MFO fleet'!D19</f>
+        <f>+'MDO fleet'!D19</f>
         <v>0</v>
       </c>
       <c r="E17">
-        <f>+'MFO fleet'!E19</f>
+        <f>+'MDO fleet'!E19</f>
         <v>0</v>
       </c>
       <c r="F17">
-        <f>+'MFO fleet'!F19</f>
+        <f>+'MDO fleet'!F19</f>
         <v>0</v>
       </c>
       <c r="G17">
-        <f>+'MFO fleet'!G19</f>
+        <f>+'MDO fleet'!G19</f>
         <v>0</v>
       </c>
       <c r="H17">
@@ -6524,23 +6524,23 @@
         <v>2025</v>
       </c>
       <c r="C18">
-        <f>+'MFO fleet'!C20</f>
+        <f>+'MDO fleet'!C20</f>
         <v>0</v>
       </c>
       <c r="D18">
-        <f>+'MFO fleet'!D20</f>
+        <f>+'MDO fleet'!D20</f>
         <v>0</v>
       </c>
       <c r="E18">
-        <f>+'MFO fleet'!E20</f>
+        <f>+'MDO fleet'!E20</f>
         <v>0</v>
       </c>
       <c r="F18">
-        <f>+'MFO fleet'!F20</f>
+        <f>+'MDO fleet'!F20</f>
         <v>0</v>
       </c>
       <c r="G18">
-        <f>+'MFO fleet'!G20</f>
+        <f>+'MDO fleet'!G20</f>
         <v>0</v>
       </c>
       <c r="H18">
@@ -6670,23 +6670,23 @@
         <v>2026</v>
       </c>
       <c r="C19">
-        <f>+'MFO fleet'!C21</f>
+        <f>+'MDO fleet'!C21</f>
         <v>0</v>
       </c>
       <c r="D19">
-        <f>+'MFO fleet'!D21</f>
+        <f>+'MDO fleet'!D21</f>
         <v>0</v>
       </c>
       <c r="E19">
-        <f>+'MFO fleet'!E21</f>
+        <f>+'MDO fleet'!E21</f>
         <v>0</v>
       </c>
       <c r="F19">
-        <f>+'MFO fleet'!F21</f>
+        <f>+'MDO fleet'!F21</f>
         <v>0</v>
       </c>
       <c r="G19">
-        <f>+'MFO fleet'!G21</f>
+        <f>+'MDO fleet'!G21</f>
         <v>0</v>
       </c>
       <c r="H19">
@@ -6816,23 +6816,23 @@
         <v>2027</v>
       </c>
       <c r="C20">
-        <f>+'MFO fleet'!C22</f>
+        <f>+'MDO fleet'!C22</f>
         <v>0</v>
       </c>
       <c r="D20">
-        <f>+'MFO fleet'!D22</f>
+        <f>+'MDO fleet'!D22</f>
         <v>0</v>
       </c>
       <c r="E20">
-        <f>+'MFO fleet'!E22</f>
+        <f>+'MDO fleet'!E22</f>
         <v>0</v>
       </c>
       <c r="F20">
-        <f>+'MFO fleet'!F22</f>
+        <f>+'MDO fleet'!F22</f>
         <v>0</v>
       </c>
       <c r="G20">
-        <f>+'MFO fleet'!G22</f>
+        <f>+'MDO fleet'!G22</f>
         <v>0</v>
       </c>
       <c r="H20">
@@ -6962,23 +6962,23 @@
         <v>2028</v>
       </c>
       <c r="C21">
-        <f>+'MFO fleet'!C23</f>
+        <f>+'MDO fleet'!C23</f>
         <v>0</v>
       </c>
       <c r="D21">
-        <f>+'MFO fleet'!D23</f>
+        <f>+'MDO fleet'!D23</f>
         <v>0</v>
       </c>
       <c r="E21">
-        <f>+'MFO fleet'!E23</f>
+        <f>+'MDO fleet'!E23</f>
         <v>0</v>
       </c>
       <c r="F21">
-        <f>+'MFO fleet'!F23</f>
+        <f>+'MDO fleet'!F23</f>
         <v>0</v>
       </c>
       <c r="G21">
-        <f>+'MFO fleet'!G23</f>
+        <f>+'MDO fleet'!G23</f>
         <v>0</v>
       </c>
       <c r="H21">
@@ -7108,23 +7108,23 @@
         <v>2029</v>
       </c>
       <c r="C22">
-        <f>+'MFO fleet'!C24</f>
+        <f>+'MDO fleet'!C24</f>
         <v>0</v>
       </c>
       <c r="D22">
-        <f>+'MFO fleet'!D24</f>
+        <f>+'MDO fleet'!D24</f>
         <v>0</v>
       </c>
       <c r="E22">
-        <f>+'MFO fleet'!E24</f>
+        <f>+'MDO fleet'!E24</f>
         <v>0</v>
       </c>
       <c r="F22">
-        <f>+'MFO fleet'!F24</f>
+        <f>+'MDO fleet'!F24</f>
         <v>0</v>
       </c>
       <c r="G22">
-        <f>+'MFO fleet'!G24</f>
+        <f>+'MDO fleet'!G24</f>
         <v>0</v>
       </c>
       <c r="H22">
@@ -7254,23 +7254,23 @@
         <v>2030</v>
       </c>
       <c r="C23">
-        <f>+'MFO fleet'!C25</f>
+        <f>+'MDO fleet'!C25</f>
         <v>0</v>
       </c>
       <c r="D23">
-        <f>+'MFO fleet'!D25</f>
+        <f>+'MDO fleet'!D25</f>
         <v>0</v>
       </c>
       <c r="E23">
-        <f>+'MFO fleet'!E25</f>
+        <f>+'MDO fleet'!E25</f>
         <v>0</v>
       </c>
       <c r="F23">
-        <f>+'MFO fleet'!F25</f>
+        <f>+'MDO fleet'!F25</f>
         <v>0</v>
       </c>
       <c r="G23">
-        <f>+'MFO fleet'!G25</f>
+        <f>+'MDO fleet'!G25</f>
         <v>0</v>
       </c>
       <c r="H23">
@@ -7400,23 +7400,23 @@
         <v>2031</v>
       </c>
       <c r="C24">
-        <f>+'MFO fleet'!C26</f>
+        <f>+'MDO fleet'!C26</f>
         <v>0</v>
       </c>
       <c r="D24">
-        <f>+'MFO fleet'!D26</f>
+        <f>+'MDO fleet'!D26</f>
         <v>0</v>
       </c>
       <c r="E24">
-        <f>+'MFO fleet'!E26</f>
+        <f>+'MDO fleet'!E26</f>
         <v>0</v>
       </c>
       <c r="F24">
-        <f>+'MFO fleet'!F26</f>
+        <f>+'MDO fleet'!F26</f>
         <v>0</v>
       </c>
       <c r="G24">
-        <f>+'MFO fleet'!G26</f>
+        <f>+'MDO fleet'!G26</f>
         <v>0</v>
       </c>
       <c r="H24">
@@ -7546,23 +7546,23 @@
         <v>2032</v>
       </c>
       <c r="C25">
-        <f>+'MFO fleet'!C27</f>
+        <f>+'MDO fleet'!C27</f>
         <v>0</v>
       </c>
       <c r="D25">
-        <f>+'MFO fleet'!D27</f>
+        <f>+'MDO fleet'!D27</f>
         <v>0</v>
       </c>
       <c r="E25">
-        <f>+'MFO fleet'!E27</f>
+        <f>+'MDO fleet'!E27</f>
         <v>0</v>
       </c>
       <c r="F25">
-        <f>+'MFO fleet'!F27</f>
+        <f>+'MDO fleet'!F27</f>
         <v>0</v>
       </c>
       <c r="G25">
-        <f>+'MFO fleet'!G27</f>
+        <f>+'MDO fleet'!G27</f>
         <v>0</v>
       </c>
       <c r="H25">
@@ -7692,23 +7692,23 @@
         <v>2033</v>
       </c>
       <c r="C26">
-        <f>+'MFO fleet'!C28</f>
+        <f>+'MDO fleet'!C28</f>
         <v>0</v>
       </c>
       <c r="D26">
-        <f>+'MFO fleet'!D28</f>
+        <f>+'MDO fleet'!D28</f>
         <v>0</v>
       </c>
       <c r="E26">
-        <f>+'MFO fleet'!E28</f>
+        <f>+'MDO fleet'!E28</f>
         <v>0</v>
       </c>
       <c r="F26">
-        <f>+'MFO fleet'!F28</f>
+        <f>+'MDO fleet'!F28</f>
         <v>0</v>
       </c>
       <c r="G26">
-        <f>+'MFO fleet'!G28</f>
+        <f>+'MDO fleet'!G28</f>
         <v>0</v>
       </c>
       <c r="H26">
@@ -7838,23 +7838,23 @@
         <v>2034</v>
       </c>
       <c r="C27">
-        <f>+'MFO fleet'!C29</f>
+        <f>+'MDO fleet'!C29</f>
         <v>0</v>
       </c>
       <c r="D27">
-        <f>+'MFO fleet'!D29</f>
+        <f>+'MDO fleet'!D29</f>
         <v>0</v>
       </c>
       <c r="E27">
-        <f>+'MFO fleet'!E29</f>
+        <f>+'MDO fleet'!E29</f>
         <v>0</v>
       </c>
       <c r="F27">
-        <f>+'MFO fleet'!F29</f>
+        <f>+'MDO fleet'!F29</f>
         <v>0</v>
       </c>
       <c r="G27">
-        <f>+'MFO fleet'!G29</f>
+        <f>+'MDO fleet'!G29</f>
         <v>0</v>
       </c>
       <c r="H27">
@@ -7984,23 +7984,23 @@
         <v>2035</v>
       </c>
       <c r="C28">
-        <f>+'MFO fleet'!C30</f>
+        <f>+'MDO fleet'!C30</f>
         <v>0</v>
       </c>
       <c r="D28">
-        <f>+'MFO fleet'!D30</f>
+        <f>+'MDO fleet'!D30</f>
         <v>0</v>
       </c>
       <c r="E28">
-        <f>+'MFO fleet'!E30</f>
+        <f>+'MDO fleet'!E30</f>
         <v>0</v>
       </c>
       <c r="F28">
-        <f>+'MFO fleet'!F30</f>
+        <f>+'MDO fleet'!F30</f>
         <v>0</v>
       </c>
       <c r="G28">
-        <f>+'MFO fleet'!G30</f>
+        <f>+'MDO fleet'!G30</f>
         <v>0</v>
       </c>
       <c r="H28">
@@ -8130,23 +8130,23 @@
         <v>2036</v>
       </c>
       <c r="C29">
-        <f>+'MFO fleet'!C31</f>
+        <f>+'MDO fleet'!C31</f>
         <v>0</v>
       </c>
       <c r="D29">
-        <f>+'MFO fleet'!D31</f>
+        <f>+'MDO fleet'!D31</f>
         <v>0</v>
       </c>
       <c r="E29">
-        <f>+'MFO fleet'!E31</f>
+        <f>+'MDO fleet'!E31</f>
         <v>0</v>
       </c>
       <c r="F29">
-        <f>+'MFO fleet'!F31</f>
+        <f>+'MDO fleet'!F31</f>
         <v>0</v>
       </c>
       <c r="G29">
-        <f>+'MFO fleet'!G31</f>
+        <f>+'MDO fleet'!G31</f>
         <v>0</v>
       </c>
       <c r="H29">
@@ -8276,23 +8276,23 @@
         <v>2037</v>
       </c>
       <c r="C30">
-        <f>+'MFO fleet'!C32</f>
+        <f>+'MDO fleet'!C32</f>
         <v>0</v>
       </c>
       <c r="D30">
-        <f>+'MFO fleet'!D32</f>
+        <f>+'MDO fleet'!D32</f>
         <v>0</v>
       </c>
       <c r="E30">
-        <f>+'MFO fleet'!E32</f>
+        <f>+'MDO fleet'!E32</f>
         <v>0</v>
       </c>
       <c r="F30">
-        <f>+'MFO fleet'!F32</f>
+        <f>+'MDO fleet'!F32</f>
         <v>0</v>
       </c>
       <c r="G30">
-        <f>+'MFO fleet'!G32</f>
+        <f>+'MDO fleet'!G32</f>
         <v>0</v>
       </c>
       <c r="H30">
@@ -8422,23 +8422,23 @@
         <v>2038</v>
       </c>
       <c r="C31">
-        <f>+'MFO fleet'!C33</f>
+        <f>+'MDO fleet'!C33</f>
         <v>0</v>
       </c>
       <c r="D31">
-        <f>+'MFO fleet'!D33</f>
+        <f>+'MDO fleet'!D33</f>
         <v>0</v>
       </c>
       <c r="E31">
-        <f>+'MFO fleet'!E33</f>
+        <f>+'MDO fleet'!E33</f>
         <v>0</v>
       </c>
       <c r="F31">
-        <f>+'MFO fleet'!F33</f>
+        <f>+'MDO fleet'!F33</f>
         <v>0</v>
       </c>
       <c r="G31">
-        <f>+'MFO fleet'!G33</f>
+        <f>+'MDO fleet'!G33</f>
         <v>0</v>
       </c>
       <c r="H31">
@@ -8568,23 +8568,23 @@
         <v>2039</v>
       </c>
       <c r="C32">
-        <f>+'MFO fleet'!C34</f>
+        <f>+'MDO fleet'!C34</f>
         <v>0</v>
       </c>
       <c r="D32">
-        <f>+'MFO fleet'!D34</f>
+        <f>+'MDO fleet'!D34</f>
         <v>0</v>
       </c>
       <c r="E32">
-        <f>+'MFO fleet'!E34</f>
+        <f>+'MDO fleet'!E34</f>
         <v>0</v>
       </c>
       <c r="F32">
-        <f>+'MFO fleet'!F34</f>
+        <f>+'MDO fleet'!F34</f>
         <v>0</v>
       </c>
       <c r="G32">
-        <f>+'MFO fleet'!G34</f>
+        <f>+'MDO fleet'!G34</f>
         <v>0</v>
       </c>
       <c r="H32">
@@ -8714,23 +8714,23 @@
         <v>2040</v>
       </c>
       <c r="C33">
-        <f>+'MFO fleet'!C35</f>
+        <f>+'MDO fleet'!C35</f>
         <v>0</v>
       </c>
       <c r="D33">
-        <f>+'MFO fleet'!D35</f>
+        <f>+'MDO fleet'!D35</f>
         <v>0</v>
       </c>
       <c r="E33">
-        <f>+'MFO fleet'!E35</f>
+        <f>+'MDO fleet'!E35</f>
         <v>0</v>
       </c>
       <c r="F33">
-        <f>+'MFO fleet'!F35</f>
+        <f>+'MDO fleet'!F35</f>
         <v>0</v>
       </c>
       <c r="G33">
-        <f>+'MFO fleet'!G35</f>
+        <f>+'MDO fleet'!G35</f>
         <v>0</v>
       </c>
       <c r="H33">
@@ -8860,23 +8860,23 @@
         <v>2041</v>
       </c>
       <c r="C34">
-        <f>+'MFO fleet'!C36</f>
+        <f>+'MDO fleet'!C36</f>
         <v>0</v>
       </c>
       <c r="D34">
-        <f>+'MFO fleet'!D36</f>
+        <f>+'MDO fleet'!D36</f>
         <v>0</v>
       </c>
       <c r="E34">
-        <f>+'MFO fleet'!E36</f>
+        <f>+'MDO fleet'!E36</f>
         <v>0</v>
       </c>
       <c r="F34">
-        <f>+'MFO fleet'!F36</f>
+        <f>+'MDO fleet'!F36</f>
         <v>0</v>
       </c>
       <c r="G34">
-        <f>+'MFO fleet'!G36</f>
+        <f>+'MDO fleet'!G36</f>
         <v>0</v>
       </c>
       <c r="H34">
@@ -9006,23 +9006,23 @@
         <v>2042</v>
       </c>
       <c r="C35">
-        <f>+'MFO fleet'!C37</f>
+        <f>+'MDO fleet'!C37</f>
         <v>0</v>
       </c>
       <c r="D35">
-        <f>+'MFO fleet'!D37</f>
+        <f>+'MDO fleet'!D37</f>
         <v>0</v>
       </c>
       <c r="E35">
-        <f>+'MFO fleet'!E37</f>
+        <f>+'MDO fleet'!E37</f>
         <v>0</v>
       </c>
       <c r="F35">
-        <f>+'MFO fleet'!F37</f>
+        <f>+'MDO fleet'!F37</f>
         <v>0</v>
       </c>
       <c r="G35">
-        <f>+'MFO fleet'!G37</f>
+        <f>+'MDO fleet'!G37</f>
         <v>0</v>
       </c>
       <c r="H35">
@@ -9152,23 +9152,23 @@
         <v>2043</v>
       </c>
       <c r="C36">
-        <f>+'MFO fleet'!C38</f>
+        <f>+'MDO fleet'!C38</f>
         <v>0</v>
       </c>
       <c r="D36">
-        <f>+'MFO fleet'!D38</f>
+        <f>+'MDO fleet'!D38</f>
         <v>0</v>
       </c>
       <c r="E36">
-        <f>+'MFO fleet'!E38</f>
+        <f>+'MDO fleet'!E38</f>
         <v>0</v>
       </c>
       <c r="F36">
-        <f>+'MFO fleet'!F38</f>
+        <f>+'MDO fleet'!F38</f>
         <v>0</v>
       </c>
       <c r="G36">
-        <f>+'MFO fleet'!G38</f>
+        <f>+'MDO fleet'!G38</f>
         <v>0</v>
       </c>
       <c r="H36">
@@ -9298,23 +9298,23 @@
         <v>2044</v>
       </c>
       <c r="C37">
-        <f>+'MFO fleet'!C39</f>
+        <f>+'MDO fleet'!C39</f>
         <v>0</v>
       </c>
       <c r="D37">
-        <f>+'MFO fleet'!D39</f>
+        <f>+'MDO fleet'!D39</f>
         <v>0</v>
       </c>
       <c r="E37">
-        <f>+'MFO fleet'!E39</f>
+        <f>+'MDO fleet'!E39</f>
         <v>0</v>
       </c>
       <c r="F37">
-        <f>+'MFO fleet'!F39</f>
+        <f>+'MDO fleet'!F39</f>
         <v>0</v>
       </c>
       <c r="G37">
-        <f>+'MFO fleet'!G39</f>
+        <f>+'MDO fleet'!G39</f>
         <v>0</v>
       </c>
       <c r="H37">
@@ -9444,23 +9444,23 @@
         <v>2045</v>
       </c>
       <c r="C38">
-        <f>+'MFO fleet'!C40</f>
+        <f>+'MDO fleet'!C40</f>
         <v>0</v>
       </c>
       <c r="D38">
-        <f>+'MFO fleet'!D40</f>
+        <f>+'MDO fleet'!D40</f>
         <v>0</v>
       </c>
       <c r="E38">
-        <f>+'MFO fleet'!E40</f>
+        <f>+'MDO fleet'!E40</f>
         <v>0</v>
       </c>
       <c r="F38">
-        <f>+'MFO fleet'!F40</f>
+        <f>+'MDO fleet'!F40</f>
         <v>0</v>
       </c>
       <c r="G38">
-        <f>+'MFO fleet'!G40</f>
+        <f>+'MDO fleet'!G40</f>
         <v>0</v>
       </c>
       <c r="H38">
@@ -9590,23 +9590,23 @@
         <v>2046</v>
       </c>
       <c r="C39">
-        <f>+'MFO fleet'!C41</f>
+        <f>+'MDO fleet'!C41</f>
         <v>0</v>
       </c>
       <c r="D39">
-        <f>+'MFO fleet'!D41</f>
+        <f>+'MDO fleet'!D41</f>
         <v>0</v>
       </c>
       <c r="E39">
-        <f>+'MFO fleet'!E41</f>
+        <f>+'MDO fleet'!E41</f>
         <v>0</v>
       </c>
       <c r="F39">
-        <f>+'MFO fleet'!F41</f>
+        <f>+'MDO fleet'!F41</f>
         <v>0</v>
       </c>
       <c r="G39">
-        <f>+'MFO fleet'!G41</f>
+        <f>+'MDO fleet'!G41</f>
         <v>0</v>
       </c>
       <c r="H39">
@@ -9736,23 +9736,23 @@
         <v>2047</v>
       </c>
       <c r="C40">
-        <f>+'MFO fleet'!C42</f>
+        <f>+'MDO fleet'!C42</f>
         <v>0</v>
       </c>
       <c r="D40">
-        <f>+'MFO fleet'!D42</f>
+        <f>+'MDO fleet'!D42</f>
         <v>0</v>
       </c>
       <c r="E40">
-        <f>+'MFO fleet'!E42</f>
+        <f>+'MDO fleet'!E42</f>
         <v>0</v>
       </c>
       <c r="F40">
-        <f>+'MFO fleet'!F42</f>
+        <f>+'MDO fleet'!F42</f>
         <v>0</v>
       </c>
       <c r="G40">
-        <f>+'MFO fleet'!G42</f>
+        <f>+'MDO fleet'!G42</f>
         <v>0</v>
       </c>
       <c r="H40">
@@ -9882,23 +9882,23 @@
         <v>2048</v>
       </c>
       <c r="C41">
-        <f>+'MFO fleet'!C43</f>
+        <f>+'MDO fleet'!C43</f>
         <v>0</v>
       </c>
       <c r="D41">
-        <f>+'MFO fleet'!D43</f>
+        <f>+'MDO fleet'!D43</f>
         <v>0</v>
       </c>
       <c r="E41">
-        <f>+'MFO fleet'!E43</f>
+        <f>+'MDO fleet'!E43</f>
         <v>0</v>
       </c>
       <c r="F41">
-        <f>+'MFO fleet'!F43</f>
+        <f>+'MDO fleet'!F43</f>
         <v>0</v>
       </c>
       <c r="G41">
-        <f>+'MFO fleet'!G43</f>
+        <f>+'MDO fleet'!G43</f>
         <v>0</v>
       </c>
       <c r="H41">
@@ -10028,23 +10028,23 @@
         <v>2049</v>
       </c>
       <c r="C42">
-        <f>+'MFO fleet'!C44</f>
+        <f>+'MDO fleet'!C44</f>
         <v>0</v>
       </c>
       <c r="D42">
-        <f>+'MFO fleet'!D44</f>
+        <f>+'MDO fleet'!D44</f>
         <v>0</v>
       </c>
       <c r="E42">
-        <f>+'MFO fleet'!E44</f>
+        <f>+'MDO fleet'!E44</f>
         <v>0</v>
       </c>
       <c r="F42">
-        <f>+'MFO fleet'!F44</f>
+        <f>+'MDO fleet'!F44</f>
         <v>0</v>
       </c>
       <c r="G42">
-        <f>+'MFO fleet'!G44</f>
+        <f>+'MDO fleet'!G44</f>
         <v>0</v>
       </c>
       <c r="H42">
@@ -10174,23 +10174,23 @@
         <v>2050</v>
       </c>
       <c r="C43">
-        <f>+'MFO fleet'!C45</f>
+        <f>+'MDO fleet'!C45</f>
         <v>0</v>
       </c>
       <c r="D43">
-        <f>+'MFO fleet'!D45</f>
+        <f>+'MDO fleet'!D45</f>
         <v>0</v>
       </c>
       <c r="E43">
-        <f>+'MFO fleet'!E45</f>
+        <f>+'MDO fleet'!E45</f>
         <v>0</v>
       </c>
       <c r="F43">
-        <f>+'MFO fleet'!F45</f>
+        <f>+'MDO fleet'!F45</f>
         <v>0</v>
       </c>
       <c r="G43">
-        <f>+'MFO fleet'!G45</f>
+        <f>+'MDO fleet'!G45</f>
         <v>0</v>
       </c>
       <c r="H43">
@@ -10320,23 +10320,23 @@
         <v>2051</v>
       </c>
       <c r="C44">
-        <f>+'MFO fleet'!C46</f>
+        <f>+'MDO fleet'!C46</f>
         <v>0</v>
       </c>
       <c r="D44">
-        <f>+'MFO fleet'!D46</f>
+        <f>+'MDO fleet'!D46</f>
         <v>0</v>
       </c>
       <c r="E44">
-        <f>+'MFO fleet'!E46</f>
+        <f>+'MDO fleet'!E46</f>
         <v>0</v>
       </c>
       <c r="F44">
-        <f>+'MFO fleet'!F46</f>
+        <f>+'MDO fleet'!F46</f>
         <v>0</v>
       </c>
       <c r="G44">
-        <f>+'MFO fleet'!G46</f>
+        <f>+'MDO fleet'!G46</f>
         <v>0</v>
       </c>
       <c r="H44">
@@ -10466,23 +10466,23 @@
         <v>2052</v>
       </c>
       <c r="C45">
-        <f>+'MFO fleet'!C47</f>
+        <f>+'MDO fleet'!C47</f>
         <v>0</v>
       </c>
       <c r="D45">
-        <f>+'MFO fleet'!D47</f>
+        <f>+'MDO fleet'!D47</f>
         <v>0</v>
       </c>
       <c r="E45">
-        <f>+'MFO fleet'!E47</f>
+        <f>+'MDO fleet'!E47</f>
         <v>0</v>
       </c>
       <c r="F45">
-        <f>+'MFO fleet'!F47</f>
+        <f>+'MDO fleet'!F47</f>
         <v>0</v>
       </c>
       <c r="G45">
-        <f>+'MFO fleet'!G47</f>
+        <f>+'MDO fleet'!G47</f>
         <v>0</v>
       </c>
       <c r="H45">
@@ -10612,23 +10612,23 @@
         <v>2053</v>
       </c>
       <c r="C46">
-        <f>+'MFO fleet'!C48</f>
+        <f>+'MDO fleet'!C48</f>
         <v>0</v>
       </c>
       <c r="D46">
-        <f>+'MFO fleet'!D48</f>
+        <f>+'MDO fleet'!D48</f>
         <v>0</v>
       </c>
       <c r="E46">
-        <f>+'MFO fleet'!E48</f>
+        <f>+'MDO fleet'!E48</f>
         <v>0</v>
       </c>
       <c r="F46">
-        <f>+'MFO fleet'!F48</f>
+        <f>+'MDO fleet'!F48</f>
         <v>0</v>
       </c>
       <c r="G46">
-        <f>+'MFO fleet'!G48</f>
+        <f>+'MDO fleet'!G48</f>
         <v>0</v>
       </c>
       <c r="H46">
@@ -10758,23 +10758,23 @@
         <v>2054</v>
       </c>
       <c r="C47">
-        <f>+'MFO fleet'!C49</f>
+        <f>+'MDO fleet'!C49</f>
         <v>0</v>
       </c>
       <c r="D47">
-        <f>+'MFO fleet'!D49</f>
+        <f>+'MDO fleet'!D49</f>
         <v>0</v>
       </c>
       <c r="E47">
-        <f>+'MFO fleet'!E49</f>
+        <f>+'MDO fleet'!E49</f>
         <v>0</v>
       </c>
       <c r="F47">
-        <f>+'MFO fleet'!F49</f>
+        <f>+'MDO fleet'!F49</f>
         <v>0</v>
       </c>
       <c r="G47">
-        <f>+'MFO fleet'!G49</f>
+        <f>+'MDO fleet'!G49</f>
         <v>0</v>
       </c>
       <c r="H47">
@@ -10904,23 +10904,23 @@
         <v>2055</v>
       </c>
       <c r="C48">
-        <f>+'MFO fleet'!C50</f>
+        <f>+'MDO fleet'!C50</f>
         <v>0</v>
       </c>
       <c r="D48">
-        <f>+'MFO fleet'!D50</f>
+        <f>+'MDO fleet'!D50</f>
         <v>0</v>
       </c>
       <c r="E48">
-        <f>+'MFO fleet'!E50</f>
+        <f>+'MDO fleet'!E50</f>
         <v>0</v>
       </c>
       <c r="F48">
-        <f>+'MFO fleet'!F50</f>
+        <f>+'MDO fleet'!F50</f>
         <v>0</v>
       </c>
       <c r="G48">
-        <f>+'MFO fleet'!G50</f>
+        <f>+'MDO fleet'!G50</f>
         <v>0</v>
       </c>
       <c r="H48">
@@ -11050,23 +11050,23 @@
         <v>2056</v>
       </c>
       <c r="C49">
-        <f>+'MFO fleet'!C51</f>
+        <f>+'MDO fleet'!C51</f>
         <v>0</v>
       </c>
       <c r="D49">
-        <f>+'MFO fleet'!D51</f>
+        <f>+'MDO fleet'!D51</f>
         <v>0</v>
       </c>
       <c r="E49">
-        <f>+'MFO fleet'!E51</f>
+        <f>+'MDO fleet'!E51</f>
         <v>0</v>
       </c>
       <c r="F49">
-        <f>+'MFO fleet'!F51</f>
+        <f>+'MDO fleet'!F51</f>
         <v>0</v>
       </c>
       <c r="G49">
-        <f>+'MFO fleet'!G51</f>
+        <f>+'MDO fleet'!G51</f>
         <v>0</v>
       </c>
       <c r="H49">
@@ -11196,23 +11196,23 @@
         <v>2057</v>
       </c>
       <c r="C50">
-        <f>+'MFO fleet'!C52</f>
+        <f>+'MDO fleet'!C52</f>
         <v>0</v>
       </c>
       <c r="D50">
-        <f>+'MFO fleet'!D52</f>
+        <f>+'MDO fleet'!D52</f>
         <v>0</v>
       </c>
       <c r="E50">
-        <f>+'MFO fleet'!E52</f>
+        <f>+'MDO fleet'!E52</f>
         <v>0</v>
       </c>
       <c r="F50">
-        <f>+'MFO fleet'!F52</f>
+        <f>+'MDO fleet'!F52</f>
         <v>0</v>
       </c>
       <c r="G50">
-        <f>+'MFO fleet'!G52</f>
+        <f>+'MDO fleet'!G52</f>
         <v>0</v>
       </c>
       <c r="H50">
@@ -11342,23 +11342,23 @@
         <v>2058</v>
       </c>
       <c r="C51">
-        <f>+'MFO fleet'!C53</f>
+        <f>+'MDO fleet'!C53</f>
         <v>0</v>
       </c>
       <c r="D51">
-        <f>+'MFO fleet'!D53</f>
+        <f>+'MDO fleet'!D53</f>
         <v>0</v>
       </c>
       <c r="E51">
-        <f>+'MFO fleet'!E53</f>
+        <f>+'MDO fleet'!E53</f>
         <v>0</v>
       </c>
       <c r="F51">
-        <f>+'MFO fleet'!F53</f>
+        <f>+'MDO fleet'!F53</f>
         <v>0</v>
       </c>
       <c r="G51">
-        <f>+'MFO fleet'!G53</f>
+        <f>+'MDO fleet'!G53</f>
         <v>0</v>
       </c>
       <c r="H51">
@@ -11488,23 +11488,23 @@
         <v>2059</v>
       </c>
       <c r="C52">
-        <f>+'MFO fleet'!C54</f>
+        <f>+'MDO fleet'!C54</f>
         <v>0</v>
       </c>
       <c r="D52">
-        <f>+'MFO fleet'!D54</f>
+        <f>+'MDO fleet'!D54</f>
         <v>0</v>
       </c>
       <c r="E52">
-        <f>+'MFO fleet'!E54</f>
+        <f>+'MDO fleet'!E54</f>
         <v>0</v>
       </c>
       <c r="F52">
-        <f>+'MFO fleet'!F54</f>
+        <f>+'MDO fleet'!F54</f>
         <v>0</v>
       </c>
       <c r="G52">
-        <f>+'MFO fleet'!G54</f>
+        <f>+'MDO fleet'!G54</f>
         <v>0</v>
       </c>
       <c r="H52">
@@ -11634,23 +11634,23 @@
         <v>2060</v>
       </c>
       <c r="C53">
-        <f>+'MFO fleet'!C55</f>
+        <f>+'MDO fleet'!C55</f>
         <v>0</v>
       </c>
       <c r="D53">
-        <f>+'MFO fleet'!D55</f>
+        <f>+'MDO fleet'!D55</f>
         <v>0</v>
       </c>
       <c r="E53">
-        <f>+'MFO fleet'!E55</f>
+        <f>+'MDO fleet'!E55</f>
         <v>0</v>
       </c>
       <c r="F53">
-        <f>+'MFO fleet'!F55</f>
+        <f>+'MDO fleet'!F55</f>
         <v>0</v>
       </c>
       <c r="G53">
-        <f>+'MFO fleet'!G55</f>
+        <f>+'MDO fleet'!G55</f>
         <v>0</v>
       </c>
       <c r="H53">
@@ -11780,23 +11780,23 @@
         <v>2061</v>
       </c>
       <c r="C54">
-        <f>+'MFO fleet'!C56</f>
+        <f>+'MDO fleet'!C56</f>
         <v>0</v>
       </c>
       <c r="D54">
-        <f>+'MFO fleet'!D56</f>
+        <f>+'MDO fleet'!D56</f>
         <v>0</v>
       </c>
       <c r="E54">
-        <f>+'MFO fleet'!E56</f>
+        <f>+'MDO fleet'!E56</f>
         <v>0</v>
       </c>
       <c r="F54">
-        <f>+'MFO fleet'!F56</f>
+        <f>+'MDO fleet'!F56</f>
         <v>0</v>
       </c>
       <c r="G54">
-        <f>+'MFO fleet'!G56</f>
+        <f>+'MDO fleet'!G56</f>
         <v>0</v>
       </c>
       <c r="H54">
@@ -11926,23 +11926,23 @@
         <v>2062</v>
       </c>
       <c r="C55">
-        <f>+'MFO fleet'!C57</f>
+        <f>+'MDO fleet'!C57</f>
         <v>0</v>
       </c>
       <c r="D55">
-        <f>+'MFO fleet'!D57</f>
+        <f>+'MDO fleet'!D57</f>
         <v>0</v>
       </c>
       <c r="E55">
-        <f>+'MFO fleet'!E57</f>
+        <f>+'MDO fleet'!E57</f>
         <v>0</v>
       </c>
       <c r="F55">
-        <f>+'MFO fleet'!F57</f>
+        <f>+'MDO fleet'!F57</f>
         <v>0</v>
       </c>
       <c r="G55">
-        <f>+'MFO fleet'!G57</f>
+        <f>+'MDO fleet'!G57</f>
         <v>0</v>
       </c>
       <c r="H55">
@@ -12072,23 +12072,23 @@
         <v>2063</v>
       </c>
       <c r="C56">
-        <f>+'MFO fleet'!C58</f>
+        <f>+'MDO fleet'!C58</f>
         <v>0</v>
       </c>
       <c r="D56">
-        <f>+'MFO fleet'!D58</f>
+        <f>+'MDO fleet'!D58</f>
         <v>0</v>
       </c>
       <c r="E56">
-        <f>+'MFO fleet'!E58</f>
+        <f>+'MDO fleet'!E58</f>
         <v>0</v>
       </c>
       <c r="F56">
-        <f>+'MFO fleet'!F58</f>
+        <f>+'MDO fleet'!F58</f>
         <v>0</v>
       </c>
       <c r="G56">
-        <f>+'MFO fleet'!G58</f>
+        <f>+'MDO fleet'!G58</f>
         <v>0</v>
       </c>
       <c r="H56">
@@ -12218,23 +12218,23 @@
         <v>2064</v>
       </c>
       <c r="C57">
-        <f>+'MFO fleet'!C59</f>
+        <f>+'MDO fleet'!C59</f>
         <v>0</v>
       </c>
       <c r="D57">
-        <f>+'MFO fleet'!D59</f>
+        <f>+'MDO fleet'!D59</f>
         <v>0</v>
       </c>
       <c r="E57">
-        <f>+'MFO fleet'!E59</f>
+        <f>+'MDO fleet'!E59</f>
         <v>0</v>
       </c>
       <c r="F57">
-        <f>+'MFO fleet'!F59</f>
+        <f>+'MDO fleet'!F59</f>
         <v>0</v>
       </c>
       <c r="G57">
-        <f>+'MFO fleet'!G59</f>
+        <f>+'MDO fleet'!G59</f>
         <v>0</v>
       </c>
       <c r="H57">
@@ -12364,23 +12364,23 @@
         <v>2065</v>
       </c>
       <c r="C58">
-        <f>+'MFO fleet'!C60</f>
+        <f>+'MDO fleet'!C60</f>
         <v>0</v>
       </c>
       <c r="D58">
-        <f>+'MFO fleet'!D60</f>
+        <f>+'MDO fleet'!D60</f>
         <v>0</v>
       </c>
       <c r="E58">
-        <f>+'MFO fleet'!E60</f>
+        <f>+'MDO fleet'!E60</f>
         <v>0</v>
       </c>
       <c r="F58">
-        <f>+'MFO fleet'!F60</f>
+        <f>+'MDO fleet'!F60</f>
         <v>0</v>
       </c>
       <c r="G58">
-        <f>+'MFO fleet'!G60</f>
+        <f>+'MDO fleet'!G60</f>
         <v>0</v>
       </c>
       <c r="H58">
@@ -12510,23 +12510,23 @@
         <v>2066</v>
       </c>
       <c r="C59">
-        <f>+'MFO fleet'!C61</f>
+        <f>+'MDO fleet'!C61</f>
         <v>0</v>
       </c>
       <c r="D59">
-        <f>+'MFO fleet'!D61</f>
+        <f>+'MDO fleet'!D61</f>
         <v>0</v>
       </c>
       <c r="E59">
-        <f>+'MFO fleet'!E61</f>
+        <f>+'MDO fleet'!E61</f>
         <v>0</v>
       </c>
       <c r="F59">
-        <f>+'MFO fleet'!F61</f>
+        <f>+'MDO fleet'!F61</f>
         <v>0</v>
       </c>
       <c r="G59">
-        <f>+'MFO fleet'!G61</f>
+        <f>+'MDO fleet'!G61</f>
         <v>0</v>
       </c>
       <c r="H59">
@@ -12656,23 +12656,23 @@
         <v>2067</v>
       </c>
       <c r="C60">
-        <f>+'MFO fleet'!C62</f>
+        <f>+'MDO fleet'!C62</f>
         <v>0</v>
       </c>
       <c r="D60">
-        <f>+'MFO fleet'!D62</f>
+        <f>+'MDO fleet'!D62</f>
         <v>0</v>
       </c>
       <c r="E60">
-        <f>+'MFO fleet'!E62</f>
+        <f>+'MDO fleet'!E62</f>
         <v>0</v>
       </c>
       <c r="F60">
-        <f>+'MFO fleet'!F62</f>
+        <f>+'MDO fleet'!F62</f>
         <v>0</v>
       </c>
       <c r="G60">
-        <f>+'MFO fleet'!G62</f>
+        <f>+'MDO fleet'!G62</f>
         <v>0</v>
       </c>
       <c r="H60">
@@ -12802,23 +12802,23 @@
         <v>2068</v>
       </c>
       <c r="C61">
-        <f>+'MFO fleet'!C63</f>
+        <f>+'MDO fleet'!C63</f>
         <v>0</v>
       </c>
       <c r="D61">
-        <f>+'MFO fleet'!D63</f>
+        <f>+'MDO fleet'!D63</f>
         <v>0</v>
       </c>
       <c r="E61">
-        <f>+'MFO fleet'!E63</f>
+        <f>+'MDO fleet'!E63</f>
         <v>0</v>
       </c>
       <c r="F61">
-        <f>+'MFO fleet'!F63</f>
+        <f>+'MDO fleet'!F63</f>
         <v>0</v>
       </c>
       <c r="G61">
-        <f>+'MFO fleet'!G63</f>
+        <f>+'MDO fleet'!G63</f>
         <v>0</v>
       </c>
       <c r="H61">
@@ -12948,23 +12948,23 @@
         <v>2069</v>
       </c>
       <c r="C62">
-        <f>+'MFO fleet'!C64</f>
+        <f>+'MDO fleet'!C64</f>
         <v>0</v>
       </c>
       <c r="D62">
-        <f>+'MFO fleet'!D64</f>
+        <f>+'MDO fleet'!D64</f>
         <v>0</v>
       </c>
       <c r="E62">
-        <f>+'MFO fleet'!E64</f>
+        <f>+'MDO fleet'!E64</f>
         <v>0</v>
       </c>
       <c r="F62">
-        <f>+'MFO fleet'!F64</f>
+        <f>+'MDO fleet'!F64</f>
         <v>0</v>
       </c>
       <c r="G62">
-        <f>+'MFO fleet'!G64</f>
+        <f>+'MDO fleet'!G64</f>
         <v>0</v>
       </c>
       <c r="H62">
@@ -13094,23 +13094,23 @@
         <v>2070</v>
       </c>
       <c r="C63">
-        <f>+'MFO fleet'!C65</f>
+        <f>+'MDO fleet'!C65</f>
         <v>0</v>
       </c>
       <c r="D63">
-        <f>+'MFO fleet'!D65</f>
+        <f>+'MDO fleet'!D65</f>
         <v>0</v>
       </c>
       <c r="E63">
-        <f>+'MFO fleet'!E65</f>
+        <f>+'MDO fleet'!E65</f>
         <v>0</v>
       </c>
       <c r="F63">
-        <f>+'MFO fleet'!F65</f>
+        <f>+'MDO fleet'!F65</f>
         <v>0</v>
       </c>
       <c r="G63">
-        <f>+'MFO fleet'!G65</f>
+        <f>+'MDO fleet'!G65</f>
         <v>0</v>
       </c>
       <c r="H63">
@@ -13240,23 +13240,23 @@
         <v>2071</v>
       </c>
       <c r="C64">
-        <f>+'MFO fleet'!C66</f>
+        <f>+'MDO fleet'!C66</f>
         <v>0</v>
       </c>
       <c r="D64">
-        <f>+'MFO fleet'!D66</f>
+        <f>+'MDO fleet'!D66</f>
         <v>0</v>
       </c>
       <c r="E64">
-        <f>+'MFO fleet'!E66</f>
+        <f>+'MDO fleet'!E66</f>
         <v>0</v>
       </c>
       <c r="F64">
-        <f>+'MFO fleet'!F66</f>
+        <f>+'MDO fleet'!F66</f>
         <v>0</v>
       </c>
       <c r="G64">
-        <f>+'MFO fleet'!G66</f>
+        <f>+'MDO fleet'!G66</f>
         <v>0</v>
       </c>
       <c r="H64">
@@ -13386,23 +13386,23 @@
         <v>2072</v>
       </c>
       <c r="C65">
-        <f>+'MFO fleet'!C67</f>
+        <f>+'MDO fleet'!C67</f>
         <v>0</v>
       </c>
       <c r="D65">
-        <f>+'MFO fleet'!D67</f>
+        <f>+'MDO fleet'!D67</f>
         <v>0</v>
       </c>
       <c r="E65">
-        <f>+'MFO fleet'!E67</f>
+        <f>+'MDO fleet'!E67</f>
         <v>0</v>
       </c>
       <c r="F65">
-        <f>+'MFO fleet'!F67</f>
+        <f>+'MDO fleet'!F67</f>
         <v>0</v>
       </c>
       <c r="G65">
-        <f>+'MFO fleet'!G67</f>
+        <f>+'MDO fleet'!G67</f>
         <v>0</v>
       </c>
       <c r="H65">
@@ -13532,23 +13532,23 @@
         <v>2073</v>
       </c>
       <c r="C66">
-        <f>+'MFO fleet'!C68</f>
+        <f>+'MDO fleet'!C68</f>
         <v>0</v>
       </c>
       <c r="D66">
-        <f>+'MFO fleet'!D68</f>
+        <f>+'MDO fleet'!D68</f>
         <v>0</v>
       </c>
       <c r="E66">
-        <f>+'MFO fleet'!E68</f>
+        <f>+'MDO fleet'!E68</f>
         <v>0</v>
       </c>
       <c r="F66">
-        <f>+'MFO fleet'!F68</f>
+        <f>+'MDO fleet'!F68</f>
         <v>0</v>
       </c>
       <c r="G66">
-        <f>+'MFO fleet'!G68</f>
+        <f>+'MDO fleet'!G68</f>
         <v>0</v>
       </c>
       <c r="H66">
@@ -13678,23 +13678,23 @@
         <v>2074</v>
       </c>
       <c r="C67">
-        <f>+'MFO fleet'!C69</f>
+        <f>+'MDO fleet'!C69</f>
         <v>0</v>
       </c>
       <c r="D67">
-        <f>+'MFO fleet'!D69</f>
+        <f>+'MDO fleet'!D69</f>
         <v>0</v>
       </c>
       <c r="E67">
-        <f>+'MFO fleet'!E69</f>
+        <f>+'MDO fleet'!E69</f>
         <v>0</v>
       </c>
       <c r="F67">
-        <f>+'MFO fleet'!F69</f>
+        <f>+'MDO fleet'!F69</f>
         <v>0</v>
       </c>
       <c r="G67">
-        <f>+'MFO fleet'!G69</f>
+        <f>+'MDO fleet'!G69</f>
         <v>0</v>
       </c>
       <c r="H67">
@@ -13824,23 +13824,23 @@
         <v>2075</v>
       </c>
       <c r="C68">
-        <f>+'MFO fleet'!C70</f>
+        <f>+'MDO fleet'!C70</f>
         <v>0</v>
       </c>
       <c r="D68">
-        <f>+'MFO fleet'!D70</f>
+        <f>+'MDO fleet'!D70</f>
         <v>0</v>
       </c>
       <c r="E68">
-        <f>+'MFO fleet'!E70</f>
+        <f>+'MDO fleet'!E70</f>
         <v>0</v>
       </c>
       <c r="F68">
-        <f>+'MFO fleet'!F70</f>
+        <f>+'MDO fleet'!F70</f>
         <v>0</v>
       </c>
       <c r="G68">
-        <f>+'MFO fleet'!G70</f>
+        <f>+'MDO fleet'!G70</f>
         <v>0</v>
       </c>
       <c r="H68">
@@ -13973,185 +13973,185 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B3:B37"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B3" sqref="B3:B37"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B8" sqref="B8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
     <row r="3" spans="2:2">
       <c r="B3" t="s">
-        <v>94</v>
+        <v>130</v>
       </c>
     </row>
     <row r="4" spans="2:2">
       <c r="B4" t="s">
-        <v>95</v>
+        <v>131</v>
       </c>
     </row>
     <row r="5" spans="2:2">
       <c r="B5" t="s">
-        <v>96</v>
+        <v>132</v>
       </c>
     </row>
     <row r="6" spans="2:2">
       <c r="B6" t="s">
-        <v>97</v>
+        <v>133</v>
       </c>
     </row>
     <row r="7" spans="2:2">
       <c r="B7" t="s">
-        <v>98</v>
+        <v>134</v>
       </c>
     </row>
     <row r="8" spans="2:2">
       <c r="B8" t="s">
-        <v>99</v>
+        <v>94</v>
       </c>
     </row>
     <row r="9" spans="2:2">
       <c r="B9" t="s">
-        <v>100</v>
+        <v>95</v>
       </c>
     </row>
     <row r="10" spans="2:2">
       <c r="B10" t="s">
-        <v>101</v>
+        <v>96</v>
       </c>
     </row>
     <row r="11" spans="2:2">
       <c r="B11" t="s">
-        <v>102</v>
+        <v>97</v>
       </c>
     </row>
     <row r="12" spans="2:2">
       <c r="B12" t="s">
-        <v>103</v>
+        <v>98</v>
       </c>
     </row>
     <row r="13" spans="2:2">
       <c r="B13" t="s">
-        <v>104</v>
+        <v>99</v>
       </c>
     </row>
     <row r="14" spans="2:2">
       <c r="B14" t="s">
-        <v>105</v>
+        <v>100</v>
       </c>
     </row>
     <row r="15" spans="2:2">
       <c r="B15" t="s">
-        <v>106</v>
+        <v>101</v>
       </c>
     </row>
     <row r="16" spans="2:2">
       <c r="B16" t="s">
-        <v>107</v>
+        <v>102</v>
       </c>
     </row>
     <row r="17" spans="2:2">
       <c r="B17" t="s">
-        <v>108</v>
+        <v>103</v>
       </c>
     </row>
     <row r="18" spans="2:2">
       <c r="B18" t="s">
-        <v>109</v>
+        <v>104</v>
       </c>
     </row>
     <row r="19" spans="2:2">
       <c r="B19" t="s">
-        <v>110</v>
+        <v>105</v>
       </c>
     </row>
     <row r="20" spans="2:2">
       <c r="B20" t="s">
-        <v>111</v>
+        <v>106</v>
       </c>
     </row>
     <row r="21" spans="2:2">
       <c r="B21" t="s">
-        <v>112</v>
+        <v>107</v>
       </c>
     </row>
     <row r="22" spans="2:2">
       <c r="B22" t="s">
-        <v>113</v>
+        <v>108</v>
       </c>
     </row>
     <row r="23" spans="2:2">
       <c r="B23" t="s">
-        <v>114</v>
+        <v>109</v>
       </c>
     </row>
     <row r="24" spans="2:2">
       <c r="B24" t="s">
-        <v>115</v>
+        <v>110</v>
       </c>
     </row>
     <row r="25" spans="2:2">
       <c r="B25" t="s">
-        <v>116</v>
+        <v>111</v>
       </c>
     </row>
     <row r="26" spans="2:2">
       <c r="B26" t="s">
-        <v>117</v>
+        <v>112</v>
       </c>
     </row>
     <row r="27" spans="2:2">
       <c r="B27" t="s">
-        <v>118</v>
+        <v>113</v>
       </c>
     </row>
     <row r="28" spans="2:2">
       <c r="B28" t="s">
-        <v>119</v>
+        <v>114</v>
       </c>
     </row>
     <row r="29" spans="2:2">
       <c r="B29" t="s">
-        <v>120</v>
+        <v>115</v>
       </c>
     </row>
     <row r="30" spans="2:2">
       <c r="B30" t="s">
-        <v>121</v>
+        <v>116</v>
       </c>
     </row>
     <row r="31" spans="2:2">
       <c r="B31" t="s">
-        <v>122</v>
+        <v>117</v>
       </c>
     </row>
     <row r="32" spans="2:2">
       <c r="B32" t="s">
-        <v>123</v>
+        <v>118</v>
       </c>
     </row>
     <row r="33" spans="2:2">
       <c r="B33" t="s">
-        <v>124</v>
+        <v>119</v>
       </c>
     </row>
     <row r="34" spans="2:2">
       <c r="B34" t="s">
-        <v>125</v>
+        <v>120</v>
       </c>
     </row>
     <row r="35" spans="2:2">
       <c r="B35" t="s">
-        <v>126</v>
+        <v>121</v>
       </c>
     </row>
     <row r="36" spans="2:2">
       <c r="B36" t="s">
-        <v>127</v>
+        <v>122</v>
       </c>
     </row>
     <row r="37" spans="2:2">
       <c r="B37" t="s">
-        <v>128</v>
+        <v>123</v>
       </c>
     </row>
   </sheetData>
@@ -15003,7 +15003,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B4:G70"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C6" sqref="C6:C14"/>
     </sheetView>
   </sheetViews>
@@ -24523,7 +24523,7 @@
         <v>74</v>
       </c>
       <c r="Z31" s="1" t="s">
-        <v>134</v>
+        <v>129</v>
       </c>
     </row>
     <row r="32" spans="2:31">
@@ -26769,7 +26769,7 @@
         <v>2038</v>
       </c>
       <c r="C60" s="1">
-        <f t="shared" ref="C59:C67" si="37">+C59-(C35-C34)</f>
+        <f t="shared" ref="C60:C67" si="37">+C59-(C35-C34)</f>
         <v>2</v>
       </c>
       <c r="D60" s="1">
@@ -26785,7 +26785,7 @@
         <v>1</v>
       </c>
       <c r="G60" s="1">
-        <f t="shared" ref="G59:G67" si="38">+G59-(G35-G34)</f>
+        <f t="shared" ref="G60:G67" si="38">+G59-(G35-G34)</f>
         <v>203</v>
       </c>
       <c r="J60" s="1">

</xml_diff>